<commit_message>
quotations and General parameters endpoints created
</commit_message>
<xml_diff>
--- a/Cotizador 2023 y Pruebas.xlsx
+++ b/Cotizador 2023 y Pruebas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\AAA-Sistemas\cotizador-merch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26594234-17E3-4EE6-A719-E24D52429D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F901D3C-B454-4188-8336-0278F89E098D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="532">
   <si>
     <t>Fecha</t>
   </si>
@@ -1589,13 +1589,100 @@
     <t>Cotizaciones</t>
   </si>
   <si>
-    <t>Productos</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>Users</t>
+  </si>
+  <si>
+    <t>Cliente_id</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>productId</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>quotation</t>
+  </si>
+  <si>
+    <t>quotationId</t>
+  </si>
+  <si>
+    <t>costoSubTotalProceso</t>
+  </si>
+  <si>
+    <t>de Parametros</t>
+  </si>
+  <si>
+    <t>productUtilitie</t>
+  </si>
+  <si>
+    <t>productMinimun</t>
+  </si>
+  <si>
+    <t>kitUtilitie</t>
+  </si>
+  <si>
+    <t>kitMinimun</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>monthlyRate</t>
+  </si>
+  <si>
+    <t>utilitiesTable[]</t>
+  </si>
+  <si>
+    <t>generalParameters</t>
+  </si>
+  <si>
+    <t>upTo</t>
+  </si>
+  <si>
+    <t>const escalasUtilidades = [</t>
+  </si>
+  <si>
+    <t>        {hasta: 408, utilidad: 30 , minimo: 82},</t>
+  </si>
+  <si>
+    <t>        {hasta: 1429, utilidad: 28 , minimo: 188},</t>
+  </si>
+  <si>
+    <t>        {hasta: 2041, utilidad: 25 , minimo: 597},</t>
+  </si>
+  <si>
+    <t>        {hasta: 4082, utilidad: 22 , minimo: 729},</t>
+  </si>
+  <si>
+    <t>        {hasta: 9999999999, utilidad: 20 , minimo: 1230}</t>
+  </si>
+  <si>
+    <t>    ]</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>customerId</t>
+  </si>
+  <si>
+    <t>exchangeRate</t>
+  </si>
+  <si>
+    <t>isKit</t>
   </si>
 </sst>
 </file>
@@ -1728,6 +1815,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1739,7 +1827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1842,6 +1930,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -1929,7 +2029,7 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2308,6 +2408,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="1" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -25653,7 +25759,7 @@
   <dimension ref="A1:O991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -25672,14 +25778,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="184" t="s">
+      <c r="B1" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184" t="s">
+      <c r="C1" s="188"/>
+      <c r="D1" s="188" t="s">
         <v>491</v>
       </c>
-      <c r="E1" s="184"/>
+      <c r="E1" s="188"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -66819,8 +66925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A717493A-B794-4D1F-BA63-B4EEB528F9A3}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67620,67 +67726,573 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D4F259-0F9A-48F7-9F07-96F529FE3107}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="151" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="151" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="151" t="s">
         <v>496</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="151" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="151" t="s">
         <v>498</v>
       </c>
       <c r="B6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="151" t="s">
+        <v>518</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="67" t="s">
+        <v>517</v>
+      </c>
+      <c r="D9" s="184"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="184"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="27">
+        <v>0</v>
+      </c>
+      <c r="J11" s="67" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="27">
+        <v>408.16734693877549</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="27">
+        <v>81.632653061224488</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="27">
+        <v>81.632653061224488</v>
+      </c>
+      <c r="J12" s="67" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="27">
+        <v>1428.5755102040816</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E13" s="27">
+        <v>122</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="27">
+        <v>122</v>
+      </c>
+      <c r="J13" s="67" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="27">
+        <v>2040.8204081632653</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="27">
+        <v>400</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G14" s="27">
+        <v>400</v>
+      </c>
+      <c r="J14" s="67" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="27">
+        <v>4082</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.22</v>
+      </c>
+      <c r="E15" s="27">
+        <v>510</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="G15" s="27">
+        <v>510</v>
+      </c>
+      <c r="J15" s="67" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="27">
+        <v>5470</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="27">
+        <v>898</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.22</v>
+      </c>
+      <c r="G16" s="27">
+        <v>898</v>
+      </c>
+      <c r="J16" s="67" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="27">
+        <v>99999999</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.18</v>
+      </c>
+      <c r="E17" s="27">
+        <v>1094</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="27">
+        <v>1094</v>
+      </c>
+      <c r="J17" s="67" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="67" t="s">
+        <v>516</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>507</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="21"/>
+      <c r="B26" s="67" t="s">
+        <v>503</v>
+      </c>
+      <c r="C26" s="151"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="C27" s="168">
+        <v>45715</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="67" t="s">
+        <v>529</v>
+      </c>
+      <c r="C28" s="186" t="s">
+        <v>479</v>
+      </c>
+      <c r="D28" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C29" s="67" t="s">
+        <v>462</v>
+      </c>
+      <c r="D29" s="186" t="s">
+        <v>480</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="67" t="s">
+        <v>461</v>
+      </c>
+      <c r="E30" s="185">
+        <v>-15</v>
+      </c>
+      <c r="F30" s="67" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="67" t="s">
+        <v>516</v>
+      </c>
+      <c r="C31" s="185"/>
+      <c r="D31" s="67" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="67" t="s">
+        <v>527</v>
+      </c>
+      <c r="C32" s="167" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="67" t="s">
+        <v>530</v>
+      </c>
+      <c r="C33" s="164">
+        <v>1075</v>
+      </c>
+      <c r="D33" s="67" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="67" t="s">
+        <v>531</v>
+      </c>
+      <c r="C34" s="164" t="s">
+        <v>493</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="161"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>505</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>503</v>
+      </c>
+      <c r="C37" s="151"/>
+      <c r="D37" s="161"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="67" t="s">
+        <v>508</v>
+      </c>
+      <c r="C38" s="185"/>
+      <c r="D38" s="161"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>432</v>
+      </c>
+      <c r="C39" s="167">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="67" t="s">
+        <v>463</v>
+      </c>
+      <c r="C40" s="167">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C41" s="180" t="s">
+        <v>473</v>
+      </c>
+      <c r="D41" s="178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="172" t="s">
+        <v>457</v>
+      </c>
+      <c r="C42" s="179">
+        <f>+D59*D42</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="181">
+        <f>+D41/30*D32</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="166">
+        <f>+C42*$C$33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="172" t="s">
+        <v>458</v>
+      </c>
+      <c r="C43" s="24">
+        <f>+G43/$C$33</f>
+        <v>55.813953488372093</v>
+      </c>
+      <c r="E43" s="166"/>
+      <c r="G43" s="177">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="172" t="s">
+        <v>470</v>
+      </c>
+      <c r="C44" s="24">
+        <f>+G44/$C$33</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="166"/>
+      <c r="G44" s="177"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="183" t="s">
+        <v>448</v>
+      </c>
+      <c r="B45" s="67" t="s">
+        <v>456</v>
+      </c>
+      <c r="C45" s="187">
+        <f>+C42+C43</f>
+        <v>55.813953488372093</v>
+      </c>
+      <c r="G45" s="166">
+        <f>+C45*$C$33</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <f>0.5*0.2+0.5*0.15</f>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="67" t="s">
+        <v>445</v>
+      </c>
+      <c r="C47" s="24">
+        <f>IF((E72*C39)&gt;(D59+E71+C45+E74),+E76,+E77)</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="176"/>
+      <c r="F47" s="166"/>
+      <c r="G47" s="166">
+        <f>+C47*$C$33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="B49" s="21" t="s">
         <v>440</v>
       </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="21"/>
+      <c r="B50" t="s">
+        <v>503</v>
+      </c>
+      <c r="C50" s="151"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="67" t="s">
+        <v>434</v>
+      </c>
+      <c r="C52" s="178" t="s">
+        <v>482</v>
+      </c>
+      <c r="D52" s="27"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="186" t="s">
+        <v>464</v>
+      </c>
+      <c r="D53" s="67" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="67" t="s">
+        <v>472</v>
+      </c>
+      <c r="C54" s="185">
+        <v>60</v>
+      </c>
+      <c r="D54" s="67" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="67" t="s">
+        <v>460</v>
+      </c>
+      <c r="C55" s="175">
+        <v>0</v>
+      </c>
+      <c r="D55" s="27"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="67" t="s">
+        <v>435</v>
+      </c>
+      <c r="C56" s="164">
+        <v>3123.7</v>
+      </c>
+      <c r="D56" s="187">
+        <f>+C56/$C$33</f>
+        <v>2.9057674418604651</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="183" t="s">
+        <v>485</v>
+      </c>
+      <c r="B57" s="67" t="s">
+        <v>436</v>
+      </c>
+      <c r="C57" s="164">
+        <v>0</v>
+      </c>
+      <c r="D57" s="187">
+        <f>+C57/$C$33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="172"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="183" t="s">
+        <v>447</v>
+      </c>
+      <c r="B59" s="172" t="s">
+        <v>509</v>
+      </c>
+      <c r="C59" s="166">
+        <f>+D59*$C$33</f>
+        <v>156184.99999999997</v>
+      </c>
+      <c r="D59" s="24">
+        <f>+D57+(C39*D56)</f>
+        <v>145.28837209302324</v>
+      </c>
+      <c r="F59" s="166"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>